<commit_message>
case for TSLVL in upper case. check TSLVL of ELC in items view.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_Storage.xlsx
+++ b/SubRES_TMPL/SubRES_Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A204078F-B672-416C-B0D0-8B958C6AEEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAE03F1-8C5E-4A34-A73A-8222322821D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="1410" windowWidth="20040" windowHeight="14190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="4680" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC" sheetId="4" r:id="rId1"/>
@@ -3182,7 +3182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="280">
   <si>
     <t>TechName</t>
   </si>
@@ -4019,6 +4019,9 @@
   </si>
   <si>
     <t>moved</t>
+  </si>
+  <si>
+    <t>daynite</t>
   </si>
 </sst>
 </file>
@@ -5186,8 +5189,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AK59"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="Q27" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AH45" sqref="AH45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7289,7 +7292,7 @@
       </c>
       <c r="AG45" s="127"/>
       <c r="AH45" s="125" t="s">
-        <v>90</v>
+        <v>279</v>
       </c>
       <c r="AI45" s="127"/>
       <c r="AJ45" s="127" t="s">
@@ -7537,7 +7540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>